<commit_message>
Korrekturen bzgl. JAhresarbeitsentgeltgrenze durchgeführt. Alle Tests laufen
</commit_message>
<xml_diff>
--- a/src/main/insert Sozialversicherungsdaten/1 Krankenversicherungsbeitraege.xlsx
+++ b/src/main/insert Sozialversicherungsdaten/1 Krankenversicherungsbeitraege.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_krankenversicherungsbeitraege\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D49A22-9F54-470D-AD74-0EB78FA2C5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A5C3D3-7163-4E1C-9210-1ABC0D6FD23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,12 +40,6 @@
     <t>Arbeitgeberbeitrag gesetzliche Krankenversicherung in Prozent</t>
   </si>
   <si>
-    <t>Beitragsbemessungsgrenze GKV Ost</t>
-  </si>
-  <si>
-    <t>Beitragsbemessungsgrenze GKV West</t>
-  </si>
-  <si>
     <t>Eintragungsdatum</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beitragsbemessungsgrenze GKV </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jahresarbeitsentgeltgrenze GKV </t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,10 +412,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>72453.56</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>75683.12</v>
@@ -452,10 +452,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -488,17 +488,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>